<commit_message>
Update BASE DE DADOS.NF.TESTE.Copia.xlsx
</commit_message>
<xml_diff>
--- a/BASE DE DADOS.NF.TESTE.Copia.xlsx
+++ b/BASE DE DADOS.NF.TESTE.Copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinicius.dossantos\Favorites\PYTHON\GITHUB\CODES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842238EA-C0FE-436F-B256-A42D35FB2D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A2D7C4-7D89-4EFA-B0B7-B69E227BBEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{05178968-9FA4-45D5-AE32-25AD9DD5CE71}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="20">
   <si>
     <t>CODIGO</t>
   </si>
@@ -543,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93A6678-662D-4AA3-B178-B7F734962996}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -617,210 +617,6 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
-        <v>123456</v>
-      </c>
-      <c r="B4" s="10">
-        <v>12345</v>
-      </c>
-      <c r="C4" s="13">
-        <v>10000</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
-        <v>123456</v>
-      </c>
-      <c r="B5" s="10">
-        <v>12345</v>
-      </c>
-      <c r="C5" s="13">
-        <v>2496.25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>123456</v>
-      </c>
-      <c r="B6" s="10">
-        <v>12345</v>
-      </c>
-      <c r="C6" s="13">
-        <v>5515.12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
-        <v>123456</v>
-      </c>
-      <c r="B7" s="10">
-        <v>12345</v>
-      </c>
-      <c r="C7" s="13">
-        <v>5650.77</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
-        <v>123456</v>
-      </c>
-      <c r="B8" s="10">
-        <v>12345</v>
-      </c>
-      <c r="C8" s="13">
-        <v>2647.06</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
-        <v>123456</v>
-      </c>
-      <c r="B9" s="10">
-        <v>12345</v>
-      </c>
-      <c r="C9" s="13">
-        <v>12393.22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>123456</v>
-      </c>
-      <c r="B10" s="10">
-        <v>12345</v>
-      </c>
-      <c r="C10" s="13">
-        <v>11266.56</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
-        <v>123456</v>
-      </c>
-      <c r="B11" s="10">
-        <v>12345</v>
-      </c>
-      <c r="C11" s="13">
-        <v>14000</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
-        <v>123456</v>
-      </c>
-      <c r="B12" s="10">
-        <v>12345</v>
-      </c>
-      <c r="C12" s="13">
-        <v>6800</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
-        <v>123456</v>
-      </c>
-      <c r="B13" s="10">
-        <v>12345</v>
-      </c>
-      <c r="C13" s="13">
-        <v>13500</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
-        <v>123456</v>
-      </c>
-      <c r="B14" s="10">
-        <v>12345</v>
-      </c>
-      <c r="C14" s="13">
-        <v>6751.57</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
-        <v>123456</v>
-      </c>
-      <c r="B15" s="10">
-        <v>12345</v>
-      </c>
-      <c r="C15" s="13">
-        <v>1104</v>
-      </c>
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>